<commit_message>
manual case resampling, halved bias but it's still there
</commit_message>
<xml_diff>
--- a/results/full_results_PGI.xlsx
+++ b/results/full_results_PGI.xlsx
@@ -495,10 +495,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H2" t="n">
-        <v>0.588614483962117</v>
+        <v>0.588577598665504</v>
       </c>
       <c r="I2" t="n">
-        <v>0.279000005687941</v>
+        <v>0.278240951962408</v>
       </c>
       <c r="J2" t="e">
         <v>#NUM!</v>
@@ -516,7 +516,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O2" t="n">
-        <v>0.411168919482086</v>
+        <v>0.411207907409411</v>
       </c>
     </row>
     <row r="3">
@@ -536,10 +536,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F3" t="n">
-        <v>0.604118662431175</v>
+        <v>0.60400366182116</v>
       </c>
       <c r="G3" t="n">
-        <v>0.309903922043096</v>
+        <v>0.310140672331196</v>
       </c>
       <c r="H3" t="e">
         <v>#NUM!</v>
@@ -574,13 +574,13 @@
         <v>18</v>
       </c>
       <c r="C4" t="n">
-        <v>0.638200814202682</v>
+        <v>0.638066291221125</v>
       </c>
       <c r="D4" t="n">
-        <v>0.361431344201991</v>
+        <v>0.361569411877401</v>
       </c>
       <c r="E4" t="n">
-        <v>0.999632158404674</v>
+        <v>0.999635703098526</v>
       </c>
       <c r="F4" t="e">
         <v>#NUM!</v>
@@ -595,19 +595,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J4" t="n">
-        <v>0.361564342599156</v>
+        <v>0.36170117980571</v>
       </c>
       <c r="K4" t="n">
-        <v>0.310017959560113</v>
+        <v>0.310253697948053</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0155098836696224</v>
+        <v>0.0154316848992071</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0496045768829296</v>
+        <v>0.0495067276037014</v>
       </c>
       <c r="N4" t="n">
-        <v>0.325527843229736</v>
+        <v>0.32568538284726</v>
       </c>
       <c r="O4" t="e">
         <v>#NUM!</v>
@@ -636,10 +636,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H5" t="n">
-        <v>0.87165491594103</v>
+        <v>0.871937806310243</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0873286003546245</v>
+        <v>0.0879278595061394</v>
       </c>
       <c r="J5" t="e">
         <v>#NUM!</v>
@@ -657,7 +657,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O5" t="n">
-        <v>0.128368107169633</v>
+        <v>0.128085046372583</v>
       </c>
     </row>
     <row r="6">
@@ -677,10 +677,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F6" t="n">
-        <v>0.882029154103006</v>
+        <v>0.882606928066615</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0943068558082396</v>
+        <v>0.0933282465590723</v>
       </c>
       <c r="H6" t="e">
         <v>#NUM!</v>
@@ -715,13 +715,13 @@
         <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>0.891460609668767</v>
+        <v>0.89233621196557</v>
       </c>
       <c r="D7" t="n">
-        <v>0.108565803933239</v>
+        <v>0.107689997855455</v>
       </c>
       <c r="E7" t="n">
-        <v>1.00002641360201</v>
+        <v>1.00002620982103</v>
       </c>
       <c r="F7" t="e">
         <v>#NUM!</v>
@@ -736,19 +736,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J7" t="n">
-        <v>0.108562936121761</v>
+        <v>0.107687175269545</v>
       </c>
       <c r="K7" t="n">
-        <v>0.094304364627695</v>
+        <v>0.0933258003795308</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0103739644747881</v>
+        <v>0.0106688421869644</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0198051710478729</v>
+        <v>0.0203978711030383</v>
       </c>
       <c r="N7" t="n">
-        <v>0.104678329102483</v>
+        <v>0.103994642566495</v>
       </c>
       <c r="O7" t="e">
         <v>#NUM!</v>
@@ -777,10 +777,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H8" t="n">
-        <v>0.813039030998043</v>
+        <v>0.81427089119318</v>
       </c>
       <c r="I8" t="n">
-        <v>0.109808756847134</v>
+        <v>0.10902784328245</v>
       </c>
       <c r="J8" t="e">
         <v>#NUM!</v>
@@ -798,7 +798,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O8" t="n">
-        <v>0.187212071640886</v>
+        <v>0.185982621113335</v>
       </c>
     </row>
     <row r="9">
@@ -818,10 +818,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F9" t="n">
-        <v>0.85557793655576</v>
+        <v>0.855337800394946</v>
       </c>
       <c r="G9" t="n">
-        <v>0.125033990214269</v>
+        <v>0.125183563805627</v>
       </c>
       <c r="H9" t="e">
         <v>#NUM!</v>
@@ -856,13 +856,13 @@
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>0.859934692307683</v>
+        <v>0.859701573261984</v>
       </c>
       <c r="D10" t="n">
-        <v>0.140374247570529</v>
+        <v>0.140609863257113</v>
       </c>
       <c r="E10" t="n">
-        <v>1.00030893987821</v>
+        <v>1.0003114365191</v>
       </c>
       <c r="F10" t="e">
         <v>#NUM!</v>
@@ -877,19 +877,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J10" t="n">
-        <v>0.140330893760255</v>
+        <v>0.14056608463557</v>
       </c>
       <c r="K10" t="n">
-        <v>0.12499537416605</v>
+        <v>0.125144588036474</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0425257676900634</v>
+        <v>0.0410541222646858</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0468811778806308</v>
+        <v>0.0454165364777647</v>
       </c>
       <c r="N10" t="n">
-        <v>0.167521141856114</v>
+        <v>0.16619871030116</v>
       </c>
       <c r="O10" t="e">
         <v>#NUM!</v>
@@ -918,10 +918,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H11" t="n">
-        <v>0.807288504849544</v>
+        <v>0.808662161004036</v>
       </c>
       <c r="I11" t="n">
-        <v>0.139762256724728</v>
+        <v>0.137461374945292</v>
       </c>
       <c r="J11" t="e">
         <v>#NUM!</v>
@@ -939,7 +939,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O11" t="n">
-        <v>0.19299655702324</v>
+        <v>0.191621736009115</v>
       </c>
     </row>
     <row r="12">
@@ -959,10 +959,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F12" t="n">
-        <v>0.809755641719053</v>
+        <v>0.810197271584953</v>
       </c>
       <c r="G12" t="n">
-        <v>0.151662034476406</v>
+        <v>0.151187849552119</v>
       </c>
       <c r="H12" t="e">
         <v>#NUM!</v>
@@ -997,13 +997,13 @@
         <v>18</v>
       </c>
       <c r="C13" t="n">
-        <v>0.827600841924518</v>
+        <v>0.827898351653003</v>
       </c>
       <c r="D13" t="n">
-        <v>0.172752399498568</v>
+        <v>0.172452844834897</v>
       </c>
       <c r="E13" t="n">
-        <v>1.00035324142309</v>
+        <v>1.0003511964879</v>
       </c>
       <c r="F13" t="e">
         <v>#NUM!</v>
@@ -1018,19 +1018,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J13" t="n">
-        <v>0.172691391474395</v>
+        <v>0.172392297681435</v>
       </c>
       <c r="K13" t="n">
-        <v>0.151608475160743</v>
+        <v>0.151134768609519</v>
       </c>
       <c r="L13" t="n">
-        <v>0.00246626728028136</v>
+        <v>0.00153457203766954</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0203051655488456</v>
+        <v>0.0192294383276799</v>
       </c>
       <c r="N13" t="n">
-        <v>0.154074742441025</v>
+        <v>0.152669340647188</v>
       </c>
       <c r="O13" t="e">
         <v>#NUM!</v>
@@ -1059,10 +1059,10 @@
         <v>#NUM!</v>
       </c>
       <c r="H14" t="n">
-        <v>0.798344180233955</v>
+        <v>0.798854634973577</v>
       </c>
       <c r="I14" t="n">
-        <v>0.161905432034979</v>
+        <v>0.161234111127771</v>
       </c>
       <c r="J14" t="e">
         <v>#NUM!</v>
@@ -1080,7 +1080,7 @@
         <v>#NUM!</v>
       </c>
       <c r="O14" t="n">
-        <v>0.202847648796567</v>
+        <v>0.202339734090694</v>
       </c>
     </row>
     <row r="15">
@@ -1100,10 +1100,10 @@
         <v>#NUM!</v>
       </c>
       <c r="F15" t="n">
-        <v>0.817758765249216</v>
+        <v>0.817704725280448</v>
       </c>
       <c r="G15" t="n">
-        <v>0.165530753502638</v>
+        <v>0.165582003926798</v>
       </c>
       <c r="H15" t="e">
         <v>#NUM!</v>
@@ -1138,13 +1138,13 @@
         <v>18</v>
       </c>
       <c r="C16" t="n">
-        <v>0.828638689570751</v>
+        <v>0.828573269432525</v>
       </c>
       <c r="D16" t="n">
-        <v>0.172856417501016</v>
+        <v>0.172924072006996</v>
       </c>
       <c r="E16" t="n">
-        <v>1.00149510707177</v>
+        <v>1.00149734143952</v>
       </c>
       <c r="F16" t="e">
         <v>#NUM!</v>
@@ -1159,19 +1159,19 @@
         <v>#NUM!</v>
       </c>
       <c r="J16" t="n">
-        <v>0.172598364384291</v>
+        <v>0.17266553142669</v>
       </c>
       <c r="K16" t="n">
-        <v>0.165283636849397</v>
+        <v>0.16533444054959</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0193856024537609</v>
+        <v>0.0188219080317273</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0302492844122759</v>
+        <v>0.0296742026640041</v>
       </c>
       <c r="N16" t="n">
-        <v>0.184669239303157</v>
+        <v>0.184156348581317</v>
       </c>
       <c r="O16" t="e">
         <v>#NUM!</v>
@@ -1193,10 +1193,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
@@ -1210,257 +1210,257 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="n">
-        <v>0.325527843229736</v>
+        <v>0.36170117980571</v>
       </c>
       <c r="D2" t="n">
-        <v>0.297892139481332</v>
+        <v>0.321846345256781</v>
       </c>
       <c r="E2" t="n">
-        <v>0.353163546978139</v>
+        <v>0.401556014354639</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="n">
-        <v>0.411168919482086</v>
+        <v>0.32568538284726</v>
       </c>
       <c r="D3" t="n">
-        <v>0.36593854924996</v>
+        <v>0.284428294588826</v>
       </c>
       <c r="E3" t="n">
-        <v>0.456399289714211</v>
+        <v>0.366942471105695</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="n">
-        <v>0.361564342599156</v>
+        <v>0.411207907409411</v>
       </c>
       <c r="D4" t="n">
-        <v>0.319216227892255</v>
+        <v>0.373866616526509</v>
       </c>
       <c r="E4" t="n">
-        <v>0.403912457306057</v>
+        <v>0.448549198292314</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>0.104678329102483</v>
+        <v>0.172392297681435</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0591742340392245</v>
+        <v>0.140769610086204</v>
       </c>
       <c r="E5" t="n">
-        <v>0.150182424165742</v>
+        <v>0.204014985276666</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.128368107169633</v>
+        <v>0.152669340647188</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0849534592962602</v>
+        <v>0.119133473603247</v>
       </c>
       <c r="E6" t="n">
-        <v>0.171782755043007</v>
+        <v>0.18620520769113</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>0.108562936121761</v>
+        <v>0.191621736009115</v>
       </c>
       <c r="D7" t="n">
-        <v>0.073226249241419</v>
+        <v>0.159968711699012</v>
       </c>
       <c r="E7" t="n">
-        <v>0.143899623002102</v>
+        <v>0.223274760319218</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" t="n">
-        <v>0.167521141856114</v>
+        <v>0.14056608463557</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0584782172581457</v>
+        <v>0.0661913249147279</v>
       </c>
       <c r="E8" t="n">
-        <v>0.276564066454082</v>
+        <v>0.214940844356412</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
       <c r="C9" t="n">
-        <v>0.187212071640886</v>
+        <v>0.16619871030116</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0783498850591239</v>
+        <v>0.0979678299955207</v>
       </c>
       <c r="E9" t="n">
-        <v>0.296074258222648</v>
+        <v>0.2344295906068</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
       <c r="C10" t="n">
-        <v>0.140330893760255</v>
+        <v>0.185982621113335</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0351122359018892</v>
+        <v>0.115247247965152</v>
       </c>
       <c r="E10" t="n">
-        <v>0.245549551618621</v>
+        <v>0.256717994261517</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>0.154074742441025</v>
+        <v>0.17266553142669</v>
       </c>
       <c r="D11" t="n">
-        <v>0.127876087544257</v>
+        <v>0.0918797609897858</v>
       </c>
       <c r="E11" t="n">
-        <v>0.180273397337792</v>
+        <v>0.253451301863595</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C12" t="n">
-        <v>0.19299655702324</v>
+        <v>0.184156348581317</v>
       </c>
       <c r="D12" t="n">
-        <v>0.177106966948526</v>
+        <v>0.106753355168802</v>
       </c>
       <c r="E12" t="n">
-        <v>0.208886147097955</v>
+        <v>0.261559341993832</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C13" t="n">
-        <v>0.172691391474395</v>
+        <v>0.202339734090694</v>
       </c>
       <c r="D13" t="n">
-        <v>0.156169826148935</v>
+        <v>0.131528250415873</v>
       </c>
       <c r="E13" t="n">
-        <v>0.189212956799855</v>
+        <v>0.273151217765516</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C14" t="n">
-        <v>0.184669239303157</v>
+        <v>0.107687175269545</v>
       </c>
       <c r="D14" t="n">
-        <v>0.07856947491023</v>
+        <v>0.0644074612943271</v>
       </c>
       <c r="E14" t="n">
-        <v>0.290769003696085</v>
+        <v>0.150966889244762</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C15" t="n">
-        <v>0.202847648796567</v>
+        <v>0.103994642566495</v>
       </c>
       <c r="D15" t="n">
-        <v>0.106173537312477</v>
+        <v>0.0633626210390709</v>
       </c>
       <c r="E15" t="n">
-        <v>0.299521760280657</v>
+        <v>0.14462666409392</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C16" t="n">
-        <v>0.172598364384291</v>
+        <v>0.128085046372583</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0781559065341878</v>
+        <v>0.0887273901220133</v>
       </c>
       <c r="E16" t="n">
-        <v>0.267040822234395</v>
+        <v>0.167442702623153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use available information for each outcome separately, with age filter
</commit_message>
<xml_diff>
--- a/results/full_results_PGI.xlsx
+++ b/results/full_results_PGI.xlsx
@@ -566,32 +566,32 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>0.828786046612005</v>
+        <v>0.876297854499272</v>
       </c>
       <c r="D5" t="n">
-        <v>0.171308442021467</v>
+        <v>0.123770409774205</v>
       </c>
       <c r="E5" t="n">
-        <v>1.00009448863347</v>
+        <v>1.00006826427348</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5" t="n">
-        <v>0.171292256850193</v>
+        <v>0.123761961253836</v>
       </c>
       <c r="K5" t="n">
-        <v>0.163182905907854</v>
+        <v>0.124509568960829</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0487318318534135</v>
+        <v>0.0973769302925883</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0522544724829854</v>
+        <v>0.104746416381763</v>
       </c>
       <c r="N5" t="n">
-        <v>0.211914737761267</v>
+        <v>0.221886499253417</v>
       </c>
       <c r="O5"/>
     </row>
@@ -606,10 +606,10 @@
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6" t="n">
-        <v>0.825263073132934</v>
+        <v>0.868927865337484</v>
       </c>
       <c r="G6" t="n">
-        <v>0.163198324837639</v>
+        <v>0.124518068516095</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -633,10 +633,10 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>0.776526636675322</v>
+        <v>0.771544287679496</v>
       </c>
       <c r="I7" t="n">
-        <v>0.144137902307866</v>
+        <v>0.0974932776552064</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -644,7 +644,7 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7" t="n">
-        <v>0.223546729333179</v>
+        <v>0.228508377635599</v>
       </c>
     </row>
     <row r="8">
@@ -867,10 +867,10 @@
         <v>0.363549076667738</v>
       </c>
       <c r="D2" t="n">
-        <v>0.312363504581606</v>
+        <v>0.318321444760205</v>
       </c>
       <c r="E2" t="n">
-        <v>0.414734648753871</v>
+        <v>0.408776708575272</v>
       </c>
     </row>
     <row r="3">
@@ -884,10 +884,10 @@
         <v>0.337047759615696</v>
       </c>
       <c r="D3" t="n">
-        <v>0.288251576465979</v>
+        <v>0.30718922769377</v>
       </c>
       <c r="E3" t="n">
-        <v>0.385843942765412</v>
+        <v>0.366906291537621</v>
       </c>
     </row>
     <row r="4">
@@ -901,10 +901,10 @@
         <v>0.409773067729312</v>
       </c>
       <c r="D4" t="n">
-        <v>0.362936702996371</v>
+        <v>0.369460038025135</v>
       </c>
       <c r="E4" t="n">
-        <v>0.456609432462253</v>
+        <v>0.450086097433489</v>
       </c>
     </row>
     <row r="5">
@@ -915,13 +915,13 @@
         <v>19</v>
       </c>
       <c r="C5" t="n">
-        <v>0.171292256850193</v>
+        <v>0.123761961253836</v>
       </c>
       <c r="D5" t="n">
-        <v>0.100618794235736</v>
+        <v>0.0401812406897797</v>
       </c>
       <c r="E5" t="n">
-        <v>0.241965719464651</v>
+        <v>0.207342681817893</v>
       </c>
     </row>
     <row r="6">
@@ -932,13 +932,13 @@
         <v>19</v>
       </c>
       <c r="C6" t="n">
-        <v>0.211914737761267</v>
+        <v>0.221886499253417</v>
       </c>
       <c r="D6" t="n">
-        <v>0.149533150567593</v>
+        <v>0.170564263286972</v>
       </c>
       <c r="E6" t="n">
-        <v>0.274296324954942</v>
+        <v>0.273208735219862</v>
       </c>
     </row>
     <row r="7">
@@ -949,13 +949,13 @@
         <v>19</v>
       </c>
       <c r="C7" t="n">
-        <v>0.223546729333179</v>
+        <v>0.228508377635599</v>
       </c>
       <c r="D7" t="n">
-        <v>0.161444869967394</v>
+        <v>0.169776667591906</v>
       </c>
       <c r="E7" t="n">
-        <v>0.285648588698963</v>
+        <v>0.287240087679292</v>
       </c>
     </row>
     <row r="8">
@@ -969,10 +969,10 @@
         <v>0.206647279512115</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0830390596349577</v>
+        <v>0.0654259339770781</v>
       </c>
       <c r="E8" t="n">
-        <v>0.330255499389273</v>
+        <v>0.347868625047153</v>
       </c>
     </row>
     <row r="9">
@@ -986,10 +986,10 @@
         <v>0.227222950727278</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0968587419549114</v>
+        <v>0.0888121318463161</v>
       </c>
       <c r="E9" t="n">
-        <v>0.357587159499644</v>
+        <v>0.365633769608239</v>
       </c>
     </row>
     <row r="10">
@@ -1003,10 +1003,10 @@
         <v>0.235700122406782</v>
       </c>
       <c r="D10" t="n">
-        <v>0.109922490958536</v>
+        <v>0.0985785216316375</v>
       </c>
       <c r="E10" t="n">
-        <v>0.361477753855028</v>
+        <v>0.372821723181926</v>
       </c>
     </row>
     <row r="11">
@@ -1020,10 +1020,10 @@
         <v>0.146880899506549</v>
       </c>
       <c r="D11" t="n">
-        <v>0.101338007685282</v>
+        <v>0.101101015285838</v>
       </c>
       <c r="E11" t="n">
-        <v>0.192423791327816</v>
+        <v>0.19266078372726</v>
       </c>
     </row>
     <row r="12">
@@ -1037,10 +1037,10 @@
         <v>0.151365123761325</v>
       </c>
       <c r="D12" t="n">
-        <v>0.104790119566145</v>
+        <v>0.0993945930581704</v>
       </c>
       <c r="E12" t="n">
-        <v>0.197940127956505</v>
+        <v>0.20333565446448</v>
       </c>
     </row>
     <row r="13">
@@ -1054,10 +1054,10 @@
         <v>0.169589021271622</v>
       </c>
       <c r="D13" t="n">
-        <v>0.122796806239691</v>
+        <v>0.121028809292652</v>
       </c>
       <c r="E13" t="n">
-        <v>0.216381236303552</v>
+        <v>0.218149233250591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>